<commit_message>
fix: Add updated valuesets and convert xlsx files into JSON
</commit_message>
<xml_diff>
--- a/input/vocabulary/source/2.16.840.1.113762.1.4.1130.11.xlsx
+++ b/input/vocabulary/source/2.16.840.1.113762.1.4.1130.11.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <workbookPr defaultThemeVersion="202300"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarapark/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88AF6F53-A737-4947-83E6-3C46793A268B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Value Set Info" r:id="rId3" sheetId="1"/>
-    <sheet name="Expansion List" r:id="rId4" sheetId="2"/>
+    <sheet name="Value Set Info" sheetId="1" r:id="rId1"/>
+    <sheet name="Expansion List" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">'Expansion List'!$A$14:$F$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Expansion List'!$A$13:$F$13</definedName>
   </definedNames>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -276,69 +284,35 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0"/>
-  </numFmts>
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
-      <sz val="11.0"/>
-      <b val="true"/>
+      <family val="2"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="12"/>
       <name val="Calibri"/>
-      <sz val="11.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="12"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="14.0"/>
-      <color indexed="18"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <b val="true"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="31"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -346,117 +320,18 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="22"/>
-      </patternFill>
-    </fill>
-    <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="22"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="12"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="12"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="29"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="29"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="20558A"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="20558A"/>
+        <fgColor rgb="FF20558A"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
-    </border>
-    <border>
-      <right style="thin"/>
-    </border>
-    <border>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-    </border>
-    <border>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin"/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
     </border>
     <border>
       <left style="thin">
@@ -471,81 +346,45 @@
       <bottom style="thin">
         <color indexed="8"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="16" fontId="1" fillId="3" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="true">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="8" xfId="0" applyBorder="true" applyFont="true" applyNumberFormat="true">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="5" borderId="8" xfId="0" applyBorder="true" applyFont="true" applyFill="true" applyNumberFormat="true">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="top" horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="top" horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="5" borderId="8" xfId="0" applyBorder="true" applyFont="true" applyFill="true" applyNumberFormat="true">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="left" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" horizontal="left" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
-      <alignment vertical="top" horizontal="left" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
-      <alignment horizontal="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true">
-      <alignment horizontal="right" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
-      <alignment horizontal="left" indent="1" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
-      <alignment horizontal="left" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="top" horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="top" horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="twoCell">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
@@ -560,13 +399,19 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Picture">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="true"/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -587,8 +432,8 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="twoCell">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
@@ -603,13 +448,19 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Picture">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="true"/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -629,658 +480,984 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="0E2841"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E8E8E8"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="156082"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="E97132"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="196B24"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="0F9ED5"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="A02B93"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="4EA72E"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="467886"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="96607D"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
-    <pageSetUpPr fitToPage="true" autoPageBreaks="true"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true" showGridLines="true"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" outlineLevelRow="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.0" customWidth="true"/>
-    <col min="2" max="2" width="45.0" customWidth="true"/>
-    <col min="3" max="3" width="30.0" customWidth="true"/>
-    <col min="4" max="4" width="45.0" customWidth="true"/>
-    <col min="5" max="5" width="45.0" customWidth="true"/>
+    <col min="1" max="1" width="40" customWidth="1"/>
+    <col min="2" max="2" width="45" customWidth="1"/>
+    <col min="3" max="3" width="30" customWidth="1"/>
+    <col min="4" max="5" width="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="46.0" customHeight="true">
-      <c r="A1" s="22"/>
-    </row>
-    <row r="2" ht="15.0" customHeight="true">
-      <c r="A2" s="8" t="s">
+    <row r="1" spans="1:6" ht="46" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9">
-      <c r="B9" s="8" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="s" s="8">
+    <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B11" t="s" s="12">
+      <c r="B11" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="s" s="8">
+    <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B12" t="s" s="12">
+      <c r="B12" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="s" s="8">
+    <row r="13" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B13" t="s" s="12">
+      <c r="B13" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="s" s="8">
+    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B14" t="s" s="12">
+      <c r="B14" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="s" s="8">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="12"/>
-    </row>
-    <row r="17">
-      <c r="A17" t="s" s="8">
+      <c r="B15" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" outlineLevel="1">
-      <c r="A18" t="s" s="1">
+    <row r="18" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B18" t="s" s="1">
+      <c r="B18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C18" t="s" s="1">
+      <c r="C18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D18" t="s" s="1">
+      <c r="D18" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" ht="15.0" customHeight="true" outlineLevel="1">
-      <c r="A19" t="s" s="12">
+    <row r="19" spans="1:4" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B19" t="s" s="12">
+      <c r="B19" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="20" ht="15.0" customHeight="true" outlineLevel="1">
-      <c r="A20" t="s" s="12">
+    <row r="20" spans="1:4" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B20" t="s" s="12">
+      <c r="B20" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="21" ht="15.0" customHeight="true" outlineLevel="1">
-      <c r="A21" t="s" s="12">
+    <row r="21" spans="1:4" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B21" t="s" s="12">
+      <c r="B21" s="3" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells>
+  <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
-  <printOptions gridLines="true" horizontalCentered="true"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="landscape" fitToHeight="1" fitToWidth="1"/>
+  <printOptions horizontalCentered="1" gridLines="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
-    <pageSetUpPr fitToPage="true" autoPageBreaks="true"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="true">
-      <pane ySplit="14.0" state="frozen" topLeftCell="A15" activePane="bottomLeft"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="13" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.0" customWidth="true"/>
-    <col min="2" max="2" width="80.0" customWidth="true"/>
-    <col min="3" max="3" width="20.0" customWidth="true"/>
-    <col min="4" max="4" width="25.0" customWidth="true"/>
-    <col min="5" max="5" width="30.0" customWidth="true"/>
+    <col min="1" max="1" width="35" customWidth="1"/>
+    <col min="2" max="2" width="80" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="46.0" customHeight="true">
-      <c r="A1" s="23"/>
-    </row>
-    <row r="2" ht="15.0" customHeight="true">
-      <c r="A2" s="8" t="s">
+    <row r="1" spans="1:6" ht="46" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9">
-      <c r="B9" s="8" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="s" s="8">
+    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B11" t="s" s="12">
+      <c r="B10" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="s" s="8">
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B12" t="s" s="12">
+      <c r="B11" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="s" s="8">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="s" s="1">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B14" t="s" s="1">
+      <c r="B13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C14" t="s" s="1">
+      <c r="C13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D14" t="s" s="1">
+      <c r="D13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E14" t="s" s="1">
+      <c r="E13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F14" t="s" s="1">
+      <c r="F13" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="s" s="12">
+    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B15" t="s" s="12">
+      <c r="B14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C15" t="s" s="12">
+      <c r="C14" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D15" t="s" s="12">
+      <c r="D14" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E15" t="s" s="12">
+      <c r="E14" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F15" t="s" s="12">
+      <c r="F14" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="s" s="12">
+    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B16" t="s" s="12">
+      <c r="B15" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C16" t="s" s="12">
+      <c r="C15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D16" t="s" s="12">
+      <c r="D15" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E16" t="s" s="12">
+      <c r="E15" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F16" t="s" s="12">
+      <c r="F15" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="s" s="12">
+    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B17" t="s" s="12">
+      <c r="B16" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C17" t="s" s="12">
+      <c r="C16" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D17" t="s" s="12">
+      <c r="D16" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E17" t="s" s="12">
+      <c r="E16" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F17" t="s" s="12">
+      <c r="F16" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="s" s="12">
+    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B18" t="s" s="12">
+      <c r="B17" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C18" t="s" s="12">
+      <c r="C17" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D18" t="s" s="12">
+      <c r="D17" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E18" t="s" s="12">
+      <c r="E17" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F18" t="s" s="12">
+      <c r="F17" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="s" s="12">
+    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B19" t="s" s="12">
+      <c r="B18" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C19" t="s" s="12">
+      <c r="C18" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D19" t="s" s="12">
+      <c r="D18" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E19" t="s" s="12">
+      <c r="E18" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F19" t="s" s="12">
+      <c r="F18" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="s" s="12">
+    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B20" t="s" s="12">
+      <c r="B19" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C20" t="s" s="12">
+      <c r="C19" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D20" t="s" s="12">
+      <c r="D19" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E20" t="s" s="12">
+      <c r="E19" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F20" t="s" s="12">
+      <c r="F19" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="s" s="12">
+    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B21" t="s" s="12">
+      <c r="B20" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C21" t="s" s="12">
+      <c r="C20" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D21" t="s" s="12">
+      <c r="D20" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E21" t="s" s="12">
+      <c r="E20" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F21" t="s" s="12">
+      <c r="F20" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="s" s="12">
+    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B22" t="s" s="12">
+      <c r="B21" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C22" t="s" s="12">
+      <c r="C21" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D22" t="s" s="12">
+      <c r="D21" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E22" t="s" s="12">
+      <c r="E21" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F22" t="s" s="12">
+      <c r="F21" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="s" s="12">
+    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B23" t="s" s="12">
+      <c r="B22" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C23" t="s" s="12">
+      <c r="C22" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D23" t="s" s="12">
+      <c r="D22" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E23" t="s" s="12">
+      <c r="E22" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F23" t="s" s="12">
+      <c r="F22" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="s" s="12">
+    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B24" t="s" s="12">
+      <c r="B23" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C24" t="s" s="12">
+      <c r="C23" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D24" t="s" s="12">
+      <c r="D23" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E24" t="s" s="12">
+      <c r="E23" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F24" t="s" s="12">
+      <c r="F23" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="s" s="12">
+    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B25" t="s" s="12">
+      <c r="B24" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C25" t="s" s="12">
+      <c r="C24" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D25" t="s" s="12">
+      <c r="D24" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E25" t="s" s="12">
+      <c r="E24" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F25" t="s" s="12">
+      <c r="F24" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" t="s" s="12">
+    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B26" t="s" s="12">
+      <c r="B25" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C26" t="s" s="12">
+      <c r="C25" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D26" t="s" s="12">
+      <c r="D25" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E26" t="s" s="12">
+      <c r="E25" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F26" t="s" s="12">
+      <c r="F25" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" t="s" s="12">
+    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B27" t="s" s="12">
+      <c r="B26" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C27" t="s" s="12">
+      <c r="C26" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D27" t="s" s="12">
+      <c r="D26" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E27" t="s" s="12">
+      <c r="E26" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F27" t="s" s="12">
+      <c r="F26" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" t="s" s="12">
+    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B28" t="s" s="12">
+      <c r="B27" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C28" t="s" s="12">
+      <c r="C27" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D28" t="s" s="12">
+      <c r="D27" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E28" t="s" s="12">
+      <c r="E27" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F28" t="s" s="12">
+      <c r="F27" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" t="s" s="12">
+    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B29" t="s" s="12">
+      <c r="B28" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C29" t="s" s="12">
+      <c r="C28" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D29" t="s" s="12">
+      <c r="D28" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="E29" t="s" s="12">
+      <c r="E28" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="F29" t="s" s="12">
+      <c r="F28" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" t="s" s="12">
+    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B30" t="s" s="12">
+      <c r="B29" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C30" t="s" s="12">
+      <c r="C29" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D30" t="s" s="12">
+      <c r="D29" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="E30" t="s" s="12">
+      <c r="E29" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="F30" t="s" s="12">
+      <c r="F29" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" t="s" s="12">
+    <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B31" t="s" s="12">
+      <c r="B30" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C31" t="s" s="12">
+      <c r="C30" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D31" t="s" s="12">
+      <c r="D30" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="E31" t="s" s="12">
+      <c r="E30" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="F31" t="s" s="12">
+      <c r="F30" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" t="s" s="12">
+    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B32" t="s" s="12">
+      <c r="B31" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C32" t="s" s="12">
+      <c r="C31" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D32" t="s" s="12">
+      <c r="D31" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="E32" t="s" s="12">
+      <c r="E31" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="F32" t="s" s="12">
+      <c r="F31" s="3" t="s">
         <v>56</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A14:F14"/>
-  <mergeCells>
+  <autoFilter ref="A13:F13" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
-  <printOptions gridLines="true" horizontalCentered="true"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="landscape" fitToHeight="1" fitToWidth="1"/>
+  <printOptions horizontalCentered="1" gridLines="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>